<commit_message>
Gráfico de Colunas Empilhadas
</commit_message>
<xml_diff>
--- a/7-Gráficos/07. Gráfico de Colunas Empilhadas (Parte 1) - Material(1).xlsx
+++ b/7-Gráficos/07. Gráfico de Colunas Empilhadas (Parte 1) - Material(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e775ab26b5c1cdcb/Hashtag/Aulas Excel Impressionador/Módulo 10 - Gráficos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\7-Gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB362B6-3A84-447E-8AF8-8D5FF359ACCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB369960-6D6A-406F-A5DC-3F8149D80F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico de Colunas" sheetId="1" r:id="rId1"/>
@@ -62,17 +62,31 @@
     <definedName name="Username" localSheetId="3">#REF!</definedName>
     <definedName name="Username">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Vendas</t>
   </si>
@@ -216,6 +230,9 @@
   </si>
   <si>
     <t>Ano 2020</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -419,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,6 +511,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,6 +527,1370 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Projetos Consultoria</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Projetos de BI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$E$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44409</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44440</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44470</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$E$3:$P$3</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>945</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>878</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>836</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>844</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>837</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1016</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1567</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>828</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3C2F-4C22-A5AE-43C1AEC50ED2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Projetos de Processos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$E$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44409</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44440</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44470</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$E$4:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1957</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1365</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1864</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1208</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1043</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>648</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3C2F-4C22-A5AE-43C1AEC50ED2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Projetos Jurídicos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$E$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44228</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44256</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44287</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44378</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44409</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44440</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44470</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44501</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44531</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$E$5:$P$5</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1070</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1321</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3C2F-4C22-A5AE-43C1AEC50ED2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Total</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="&quot;R$&quot;\ #,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfico de Colunas Empilhadas'!$E$6:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>"$"\ #.##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2770</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1740</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2648</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3266</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2781</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3229</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3936</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4554</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-3C2F-4C22-A5AE-43C1AEC50ED2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="2007324735"/>
+        <c:axId val="2007325215"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="2007324735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2007325215"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="2007325215"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="&quot;R$&quot;\ #,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2007324735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst>
+      <a:outerShdw blurRad="50800" dist="38100" algn="l" rotWithShape="0">
+        <a:prstClr val="black">
+          <a:alpha val="40000"/>
+        </a:prstClr>
+      </a:outerShdw>
+    </a:effectLst>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>510887</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>117763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>207818</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>103908</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C1543BC-A220-4EE3-5CEC-28FB94210D30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -776,19 +2158,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
@@ -796,7 +2178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -804,7 +2186,7 @@
         <v>5318</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -812,7 +2194,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -820,7 +2202,7 @@
         <v>5977</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -828,7 +2210,7 @@
         <v>9258</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -836,7 +2218,7 @@
         <v>8111</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -844,7 +2226,7 @@
         <v>4639</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -852,7 +2234,7 @@
         <v>6895</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -860,7 +2242,7 @@
         <v>9620</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -868,7 +2250,7 @@
         <v>7443</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -876,7 +2258,7 @@
         <v>3177</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -898,15 +2280,15 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.26953125" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
@@ -917,7 +2299,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -928,7 +2310,7 @@
         <v>9344</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -939,7 +2321,7 @@
         <v>6573</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -950,7 +2332,7 @@
         <v>7332</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -961,7 +2343,7 @@
         <v>6212</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
@@ -972,7 +2354,7 @@
         <v>5310</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
@@ -983,7 +2365,7 @@
         <v>9395</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -994,7 +2376,7 @@
         <v>4487</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +2387,7 @@
         <v>9455</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1016,7 +2398,7 @@
         <v>2192</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1027,7 +2409,7 @@
         <v>2107</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +2420,7 @@
         <v>4353</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1061,25 +2443,25 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="107" style="6" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="14" width="6.54296875" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="6"/>
+    <col min="3" max="3" width="6.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="6.5703125" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="28"/>
       <c r="D3" s="16" t="s">
         <v>37</v>
@@ -1091,7 +2473,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="15"/>
       <c r="D4" s="8" t="s">
         <v>35</v>
@@ -1103,7 +2485,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>34</v>
       </c>
@@ -1117,7 +2499,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
@@ -1131,7 +2513,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>30</v>
       </c>
@@ -1145,7 +2527,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>28</v>
       </c>
@@ -1159,7 +2541,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13"/>
       <c r="D9" s="8" t="s">
         <v>26</v>
@@ -1171,7 +2553,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
@@ -1185,7 +2567,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>23</v>
       </c>
@@ -1199,7 +2581,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
@@ -1213,7 +2595,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
       <c r="D13" s="8" t="s">
         <v>19</v>
@@ -1225,7 +2607,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>18</v>
       </c>
@@ -1239,7 +2621,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>16</v>
       </c>
@@ -1253,12 +2635,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:B3"/>
@@ -1272,18 +2654,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F946B274-1865-4279-A5EA-41A02BBB26AA}">
   <dimension ref="B1:P9"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" customWidth="1"/>
-    <col min="2" max="2" width="73.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.54296875" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
         <v>45</v>
       </c>
@@ -1327,7 +2711,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="29"/>
       <c r="D3" s="25" t="s">
         <v>44</v>
@@ -1369,7 +2753,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="29"/>
       <c r="D4" s="23" t="s">
         <v>42</v>
@@ -1411,7 +2795,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="21" t="s">
         <v>40</v>
       </c>
@@ -1452,17 +2836,68 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="30">
+        <f>SUM(E3:E5)</f>
+        <v>2770</v>
+      </c>
+      <c r="F6" s="30">
+        <f t="shared" ref="F6:P6" si="0">SUM(F3:F5)</f>
+        <v>1740</v>
+      </c>
+      <c r="G6" s="30">
+        <f t="shared" si="0"/>
+        <v>2648</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="0"/>
+        <v>2120</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="0"/>
+        <v>3266</v>
+      </c>
+      <c r="J6" s="30">
+        <f t="shared" si="0"/>
+        <v>3331</v>
+      </c>
+      <c r="K6" s="30">
+        <f t="shared" si="0"/>
+        <v>2781</v>
+      </c>
+      <c r="L6" s="30">
+        <f t="shared" si="0"/>
+        <v>3229</v>
+      </c>
+      <c r="M6" s="30">
+        <f t="shared" si="0"/>
+        <v>3936</v>
+      </c>
+      <c r="N6" s="30">
+        <f t="shared" si="0"/>
+        <v>2994</v>
+      </c>
+      <c r="O6" s="30">
+        <f t="shared" si="0"/>
+        <v>4554</v>
+      </c>
+      <c r="P6" s="30">
+        <f t="shared" si="0"/>
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>39</v>
       </c>
@@ -1480,7 +2915,7 @@
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
     </row>
-    <row r="9" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
     </row>
   </sheetData>
@@ -1488,5 +2923,6 @@
     <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>